<commit_message>
Avance en funcionalidad de miembros
Se deja lista la parte de miembros en el backend con las pruebas en postman, quedando pendiente la conexión con el frontend.
</commit_message>
<xml_diff>
--- a/docs/trim04/05_Metodologia_Agil/Epicas.xlsx
+++ b/docs/trim04/05_Metodologia_Agil/Epicas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\TaskMasterPro\docs\trim04\05_Metodologia_Agil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{673D084D-2992-4797-902C-009378757251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26FD6AB-F138-4FBE-AE20-86B4FD50D951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,9 +67,6 @@
     <t>Johan Garcia</t>
   </si>
   <si>
-    <t>Dev en curso</t>
-  </si>
-  <si>
     <t>Crítica</t>
   </si>
   <si>
@@ -107,6 +104,9 @@
   </si>
   <si>
     <t>3, 2, 2, 3, 1, 2, 1</t>
+  </si>
+  <si>
+    <t>Listo</t>
   </si>
 </sst>
 </file>
@@ -114,7 +114,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -193,12 +193,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF225091"/>
+        <fgColor rgb="FFDF2F4A"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDF2F4A"/>
+        <fgColor rgb="FF00C875"/>
       </patternFill>
     </fill>
   </fills>
@@ -208,21 +208,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF225091"/>
-      </left>
-      <right style="thick">
-        <color rgb="FF225091"/>
-      </right>
-      <top style="thick">
-        <color rgb="FF225091"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF225091"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -240,6 +225,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF00B461"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF00B461"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF00B461"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF00B461"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -258,10 +258,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -270,10 +270,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -637,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -713,23 +713,23 @@
       <c r="D4" s="6">
         <v>45717</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="G4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>18</v>
       </c>
       <c r="I4" s="7">
         <v>5</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K4" s="7">
         <v>8632698872</v>
@@ -737,10 +737,10 @@
     </row>
     <row r="5" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>21</v>
       </c>
       <c r="C5" s="6">
         <v>45705</v>
@@ -748,23 +748,23 @@
       <c r="D5" s="6">
         <v>45731</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>16</v>
-      </c>
       <c r="G5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="I5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="J5" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K5" s="7">
         <v>8881879638</v>
@@ -772,10 +772,10 @@
     </row>
     <row r="6" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="C6" s="6">
         <v>45710</v>
@@ -783,23 +783,23 @@
       <c r="D6" s="6">
         <v>45745</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>16</v>
-      </c>
       <c r="G6" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="7" t="s">
-        <v>28</v>
-      </c>
       <c r="J6" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K6" s="7">
         <v>8881898306</v>
@@ -807,10 +807,10 @@
     </row>
     <row r="7" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="5">
         <v>45705</v>
@@ -819,25 +819,25 @@
         <v>45745</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>